<commit_message>
updated ratings to reflect SA. working on simulation tab
</commit_message>
<xml_diff>
--- a/index_country.xlsx
+++ b/index_country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\Credit Rating Model Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B39ACDD3-F530-4A24-839E-7BB078CA94CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305AC99C-C3B5-4916-9D40-84076734451D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EADE75-331B-4967-8B68-39AB90716751}"/>
+    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{E7EADE75-331B-4967-8B68-39AB90716751}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>cc</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>Zambia</t>
+  </si>
+  <si>
+    <t>Algeria</t>
   </si>
 </sst>
 </file>
@@ -820,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB948CE6-9091-46B2-A0E7-EC4E56AECD96}">
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,1097 +849,1105 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>213</v>
+        <v>614</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>911</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>193</v>
+        <v>911</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>912</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>419</v>
+        <v>912</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>513</v>
+        <v>419</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>316</v>
+        <v>513</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>913</v>
+        <v>316</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>124</v>
+        <v>913</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>339</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>638</v>
+        <v>339</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>218</v>
+        <v>638</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>963</v>
+        <v>218</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>616</v>
+        <v>963</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>223</v>
+        <v>616</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>918</v>
+        <v>223</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>748</v>
+        <v>918</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>624</v>
+        <v>748</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>522</v>
+        <v>624</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>622</v>
+        <v>522</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>156</v>
+        <v>622</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>228</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>924</v>
+        <v>228</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>233</v>
+        <v>924</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>662</v>
+        <v>238</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>960</v>
+        <v>662</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>423</v>
+        <v>960</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>935</v>
+        <v>423</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>636</v>
+        <v>935</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>128</v>
+        <v>636</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>243</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>469</v>
+        <v>248</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>253</v>
+        <v>469</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>939</v>
+        <v>253</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>644</v>
+        <v>939</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>819</v>
+        <v>644</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>172</v>
+        <v>819</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>962</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>646</v>
+        <v>962</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>915</v>
+        <v>646</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>134</v>
+        <v>915</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>652</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>174</v>
+        <v>652</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>328</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>258</v>
+        <v>328</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>532</v>
+        <v>268</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>944</v>
+        <v>532</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>176</v>
+        <v>944</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>534</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>433</v>
+        <v>536</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>178</v>
+        <v>433</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>436</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>136</v>
+        <v>436</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>343</v>
+        <v>136</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>158</v>
+        <v>343</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>439</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>916</v>
+        <v>439</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>664</v>
+        <v>916</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>542</v>
+        <v>664</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>443</v>
+        <v>542</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>917</v>
+        <v>443</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>544</v>
+        <v>917</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>941</v>
+        <v>544</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>446</v>
+        <v>941</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>666</v>
+        <v>446</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>946</v>
+        <v>666</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>137</v>
+        <v>946</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>546</v>
+        <v>137</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>674</v>
+        <v>546</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>548</v>
+        <v>674</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>181</v>
+        <v>556</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>684</v>
+        <v>181</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>273</v>
+        <v>684</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>921</v>
+        <v>273</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>948</v>
+        <v>921</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>686</v>
+        <v>943</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>728</v>
+        <v>688</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>138</v>
+        <v>728</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>692</v>
+        <v>278</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>142</v>
+        <v>694</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>449</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>564</v>
+        <v>449</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>283</v>
+        <v>564</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>853</v>
+        <v>283</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>288</v>
+        <v>853</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>566</v>
+        <v>293</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>964</v>
+        <v>566</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>182</v>
+        <v>964</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>453</v>
+        <v>182</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>634</v>
+        <v>453</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>968</v>
+        <v>634</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>922</v>
+        <v>968</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>714</v>
+        <v>922</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>456</v>
+        <v>714</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>722</v>
+        <v>456</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>942</v>
+        <v>722</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>718</v>
+        <v>942</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>576</v>
+        <v>718</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>936</v>
+        <v>576</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>961</v>
+        <v>936</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>199</v>
+        <v>961</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>524</v>
+        <v>184</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>366</v>
+        <v>524</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>144</v>
+        <v>366</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>528</v>
+        <v>146</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>738</v>
+        <v>528</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>578</v>
+        <v>738</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>742</v>
+        <v>578</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>369</v>
+        <v>742</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>744</v>
+        <v>369</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>186</v>
+        <v>744</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>746</v>
+        <v>186</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>926</v>
+        <v>746</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>466</v>
+        <v>926</v>
       </c>
       <c r="B132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>112</v>
+        <v>466</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>298</v>
+        <v>111</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>927</v>
+        <v>298</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>299</v>
+        <v>927</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>582</v>
+        <v>299</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
+        <v>582</v>
+      </c>
+      <c r="B139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140">
         <v>754</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>